<commit_message>
Test case scenario exel file created and filled and README.txt file added and modified with the the repo link,
</commit_message>
<xml_diff>
--- a/TestPlan_assignment4.xlsx
+++ b/TestPlan_assignment4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aidin\OneDrive\Documents\2nd semester\Programming 2\Assignments\Assignment 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1AEF0004-4DF2-4B7D-BFC5-42685B9C8A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839FE88B-D802-48DF-9935-D90A2D662103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{EEE3B5BE-F18E-40A6-9B00-A02562CE1424}"/>
   </bookViews>
@@ -35,9 +35,212 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="66">
+  <si>
+    <t>Test Scenario</t>
+  </si>
+  <si>
+    <t>Expected Output</t>
+  </si>
+  <si>
+    <t>Add an existing player with a higher score</t>
+  </si>
+  <si>
+    <t>Entry updated successfully</t>
+  </si>
+  <si>
+    <t>Add an existing player with a lower score</t>
+  </si>
+  <si>
+    <t>Add a player with an invalid name</t>
+  </si>
+  <si>
+    <t>Error: Invalid name</t>
+  </si>
+  <si>
+    <t>Add a player with a negative score</t>
+  </si>
+  <si>
+    <t>Error: Score must be positive</t>
+  </si>
+  <si>
+    <t>Add a player with the same score as another player</t>
+  </si>
+  <si>
+    <t>Bob appears below John</t>
+  </si>
+  <si>
+    <t>Delete an existing entry</t>
+  </si>
+  <si>
+    <t>Name: John</t>
+  </si>
+  <si>
+    <t>Delete a non-existent player</t>
+  </si>
+  <si>
+    <t>Name: Steve</t>
+  </si>
+  <si>
+    <t>Error: Player not found</t>
+  </si>
+  <si>
+    <t>Name: ""</t>
+  </si>
+  <si>
+    <t>Error: Invalid input</t>
+  </si>
+  <si>
+    <t>Display leaderboard after adding entries</t>
+  </si>
+  <si>
+    <t>Entries sorted in descending order</t>
+  </si>
+  <si>
+    <t>Highlight highest score entry</t>
+  </si>
+  <si>
+    <t>Highest score visibly different</t>
+  </si>
+  <si>
+    <t>Display empty leaderboard</t>
+  </si>
+  <si>
+    <t>Save leaderboard to a file</t>
+  </si>
+  <si>
+    <t>Filename: leaderboard.csv</t>
+  </si>
+  <si>
+    <t>File saved successfully</t>
+  </si>
+  <si>
+    <t>Load leaderboard from a file</t>
+  </si>
+  <si>
+    <t>Leaderboard loaded correctly</t>
+  </si>
+  <si>
+    <t>Load from a non-existent file</t>
+  </si>
+  <si>
+    <t>Filename: missing.csv</t>
+  </si>
+  <si>
+    <t>Error: File not found</t>
+  </si>
+  <si>
+    <t>Load invalid file format</t>
+  </si>
+  <si>
+    <t>Filename: leaderboard.txt</t>
+  </si>
+  <si>
+    <t>Error: Invalid file format</t>
+  </si>
+  <si>
+    <t>Clear the leaderboard</t>
+  </si>
+  <si>
+    <t>All entries removed</t>
+  </si>
+  <si>
+    <t>Clear leaderboard when already empty</t>
+  </si>
+  <si>
+    <t>Exit without unsaved changes</t>
+  </si>
+  <si>
+    <t>Quit</t>
+  </si>
+  <si>
+    <t>Program exits</t>
+  </si>
+  <si>
+    <t>Exit with unsaved changes</t>
+  </si>
+  <si>
+    <t>Return to menu</t>
+  </si>
+  <si>
+    <t>Add a new winner with valid info</t>
+  </si>
+  <si>
+    <t>Name: John, Score: 100, Time: 2025-03-18 14:30, Sport: Soccer, Age: 25</t>
+  </si>
+  <si>
+    <t>Name: John, Score: 120, Time: 2025-03-18 14:30, Sport: Soccer, Age: 25</t>
+  </si>
+  <si>
+    <t>Name: John, Score: 90, Time: 2025-03-18 14:30, Sport: Soccer, Age: 25</t>
+  </si>
+  <si>
+    <t>Name: "", Score: 90, Time: 2025-02-23 12:50, Sport: Hockey Age: 20</t>
+  </si>
+  <si>
+    <t>Name: Alice, Score: -10, Time: 2022-10-10 14:30, Sport: Football, Age: 17</t>
+  </si>
+  <si>
+    <t>Name: Bob, Score: 100, Time: 2025-03-18 14:34, Sport: Soccer, Age: 55</t>
+  </si>
+  <si>
+    <t>Try deleting with an empty input</t>
+  </si>
+  <si>
+    <t>Input/Action</t>
+  </si>
+  <si>
+    <t>Confirm exit after message</t>
+  </si>
+  <si>
+    <t>Cancel exit after message</t>
+  </si>
+  <si>
+    <t>"Y" or "y"</t>
+  </si>
+  <si>
+    <t>"N" or "n"</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Entry added successfully and leaderboard updated</t>
+  </si>
+  <si>
+    <t>No change made and message displayed</t>
+  </si>
+  <si>
+    <t>Entry deleted and leaderboard updated</t>
+  </si>
+  <si>
+    <t>Message: Leaderboard is empty</t>
+  </si>
+  <si>
+    <t>Message: Leaderboard is already empty</t>
+  </si>
+  <si>
+    <t>Message: Unsaved changes. Confirm exit?</t>
+  </si>
+  <si>
+    <t>Success/Failure</t>
+  </si>
+  <si>
+    <t>Test Made by:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Aidin Yaseri</t>
+  </si>
+  <si>
+    <t>Program tested by:</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,16 +248,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -62,12 +285,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,12 +653,312 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{135932DE-3D20-43F7-8CC6-AA0AB0723102}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="45.85546875" customWidth="1"/>
+    <col min="2" max="2" width="63.85546875" customWidth="1"/>
+    <col min="3" max="3" width="45.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="F3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="F4" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>